<commit_message>
Update UI labels and remove unused imports
benerin UI samain bahasa, hapus import yang ga kepaka
</commit_message>
<xml_diff>
--- a/dataset/new_dataset_program.xlsx
+++ b/dataset/new_dataset_program.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TA\Program\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B410A95-9D2F-4FA9-AADB-945347F57944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882A158-29F8-4EAA-BE2D-06F01D27597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
   </sheetPr>
   <dimension ref="A1:B616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A605" workbookViewId="0">
-      <selection activeCell="E623" sqref="E623"/>
+    <sheetView tabSelected="1" topLeftCell="A582" workbookViewId="0">
+      <selection activeCell="G604" sqref="G604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>